<commit_message>
add tree edit, delete
</commit_message>
<xml_diff>
--- a/excelhere/room_one.xlsx
+++ b/excelhere/room_one.xlsx
@@ -442,21 +442,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>sadf</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>asdf</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr">
         <is>
           <t>1</t>

</xml_diff>

<commit_message>
save before add load
</commit_message>
<xml_diff>
--- a/excelhere/room_one.xlsx
+++ b/excelhere/room_one.xlsx
@@ -444,17 +444,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>hj</t>
+          <t>111</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>hjv</t>
+          <t>111</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>bhj</t>
+          <t>1</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,7 +485,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>노트</t>
+          <t>녹말요지</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -494,55 +494,13 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>600</v>
+        <v>1100</v>
       </c>
       <c r="D1" t="n">
         <v>1</v>
       </c>
       <c r="E1" t="n">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>밥공기(1)</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>6000</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>6000</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>접시100</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1000</v>
+        <v>1100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
save before check the problem
</commit_message>
<xml_diff>
--- a/excelhere/room_one.xlsx
+++ b/excelhere/room_one.xlsx
@@ -442,21 +442,9 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>111</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
+      <c r="A1" t="inlineStr"/>
+      <c r="B1" t="inlineStr"/>
+      <c r="C1" t="inlineStr"/>
       <c r="D1" t="inlineStr">
         <is>
           <t>1</t>
@@ -474,233 +462,14 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>접시100</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E1" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>종이컵</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>줄</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>1500</v>
-      </c>
-      <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="n">
-        <v>1500</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>접시140</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="n">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>에어베게</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>2600</v>
-      </c>
-      <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="n">
-        <v>2600</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>신라면(컵)</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>930</v>
-      </c>
-      <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="n">
-        <v>930</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>맥주</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>4000</v>
-      </c>
-      <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="n">
-        <v>4000</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>drink</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>ea</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-      <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>1000</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>에너지 드링크</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>캔</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>1800</t>
-        </is>
-      </c>
-      <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>1800</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>닭볶음탕</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>9000</v>
-      </c>
-      <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="n">
-        <v>9000</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>대패삼겹살</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>개</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>2000</v>
-      </c>
-      <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>